<commit_message>
Added the AI test
</commit_message>
<xml_diff>
--- a/VA01/Default.xlsx
+++ b/VA01/Default.xlsx
@@ -213,10 +213,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -526,15 +526,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="18.6015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.15625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.48046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.38671875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.6015625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.48046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.38671875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1">
+    <row r="1" ht="14.95" customFormat="1">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -549,13 +549,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>4236</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
@@ -575,7 +575,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>
@@ -594,10 +594,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>